<commit_message>
add glock zevtech slide stuff
</commit_message>
<xml_diff>
--- a/changes/556-ammo-2.xlsx
+++ b/changes/556-ammo-2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B2C27505-2847-473E-8CD9-406F2AC566FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C4AC4F-F865-43C7-9684-9DD452FD6304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{BC00A3DD-2688-4DC7-B9A4-AB624F8BC35B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>ergonomics</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>irl energy</t>
+  </si>
+  <si>
+    <t>new</t>
   </si>
 </sst>
 </file>
@@ -480,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C6E44B4-CDD7-48AE-BD69-50144A71B982}">
-  <dimension ref="A2:L14"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="146" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -491,6 +494,11 @@
     <col min="2" max="2" width="28.33203125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+    </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>23</v>

</xml_diff>